<commit_message>
Residential cover sheets updated
</commit_message>
<xml_diff>
--- a/SubRES_TMPL/SubRES_RSD-Retrofit_Trans.xlsx
+++ b/SubRES_TMPL/SubRES_RSD-Retrofit_Trans.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F42BD9-D162-4BCB-957C-98F0DE5416A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56A0B9D9-DE2B-4725-BB47-878A17987717}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="819" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{DF4C35E6-02C2-4233-84CE-A7CCAFFA4B20}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="47" r:id="rId1"/>
     <sheet name="Regions" sheetId="46" r:id="rId2"/>
     <sheet name="TechSelection" sheetId="34" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" hidden="1">#REF!</definedName>
@@ -135,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="85">
   <si>
     <t>IE</t>
   </si>
@@ -365,27 +361,15 @@
     <t>Document type:</t>
   </si>
   <si>
-    <t>Template type</t>
-  </si>
-  <si>
     <t>Sector(s):</t>
   </si>
   <si>
-    <t>Sector name</t>
-  </si>
-  <si>
     <t>Purpose:</t>
   </si>
   <si>
-    <t>Brief description of what this file is for</t>
-  </si>
-  <si>
     <t>Original developer(s):</t>
   </si>
   <si>
-    <t>Full Name(s) (Affiliation, email)</t>
-  </si>
-  <si>
     <t>Current maintainer(s):</t>
   </si>
   <si>
@@ -405,6 +389,21 @@
   </si>
   <si>
     <t>https://creativecommons.org/licenses/by-nc-sa/4.0/</t>
+  </si>
+  <si>
+    <t>New Technology</t>
+  </si>
+  <si>
+    <t>Residential sector (RSD)</t>
+  </si>
+  <si>
+    <t>Assigns new retrofit data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Olexandr Balyk ( MaREI, olexandr.balyk@ucc.ie) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jason Mc Guire ( MaREI, jason.mcguire@ucc.ie) </t>
   </si>
 </sst>
 </file>
@@ -697,9 +696,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -718,9 +714,6 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -733,14 +726,20 @@
     <xf numFmtId="164" fontId="12" fillId="6" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1103,7 +1102,7 @@
                   <a14:compatExt spid="_x0000_s89089"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-0000015C0100}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000015C0100}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1139,19 +1138,6 @@
     <mc:Fallback/>
   </mc:AlternateContent>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1478,10 +1464,9 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Z99"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1918,20 +1903,20 @@
       <c r="Z15" s="18"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="20"/>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="22"/>
-      <c r="H16" s="22"/>
-      <c r="I16" s="22"/>
-      <c r="J16" s="22"/>
-      <c r="K16" s="22"/>
-      <c r="L16" s="22"/>
+      <c r="B16" s="34"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="21"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
       <c r="M16" s="18"/>
       <c r="N16" s="18"/>
       <c r="O16" s="18"/>
@@ -1948,10 +1933,10 @@
       <c r="Z16" s="18"/>
     </row>
     <row r="17" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
+      <c r="A17" s="22"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
       <c r="E17" s="18"/>
       <c r="F17" s="18"/>
       <c r="G17" s="18"/>
@@ -1976,18 +1961,18 @@
       <c r="Z17" s="18"/>
     </row>
     <row r="18" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
-      <c r="L18" s="25"/>
+      <c r="A18" s="22"/>
+      <c r="B18" s="22"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="22"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="24"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
+      <c r="K18" s="24"/>
+      <c r="L18" s="24"/>
       <c r="M18" s="18"/>
       <c r="N18" s="18"/>
       <c r="O18" s="18"/>
@@ -2004,22 +1989,22 @@
       <c r="Z18" s="18"/>
     </row>
     <row r="19" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="26" t="s">
+      <c r="A19" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="B19" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="29"/>
-      <c r="H19" s="29"/>
-      <c r="I19" s="29"/>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
+      <c r="B19" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
+      <c r="J19" s="27"/>
+      <c r="K19" s="27"/>
+      <c r="L19" s="27"/>
       <c r="M19" s="18"/>
       <c r="N19" s="18"/>
       <c r="O19" s="18"/>
@@ -2036,22 +2021,22 @@
       <c r="Z19" s="18"/>
     </row>
     <row r="20" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="26" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="29"/>
-      <c r="H20" s="29"/>
-      <c r="I20" s="29"/>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
+      <c r="A20" s="25" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="18"/>
@@ -2068,22 +2053,22 @@
       <c r="Z20" s="18"/>
     </row>
     <row r="21" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="26" t="s">
-        <v>73</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="29"/>
-      <c r="H21" s="29"/>
-      <c r="I21" s="29"/>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
+      <c r="A21" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B21" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="27"/>
+      <c r="L21" s="27"/>
       <c r="M21" s="18"/>
       <c r="N21" s="18"/>
       <c r="O21" s="18"/>
@@ -2100,18 +2085,18 @@
       <c r="Z21" s="18"/>
     </row>
     <row r="22" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="26"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
+      <c r="A22" s="25"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="26"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
       <c r="M22" s="18"/>
       <c r="N22" s="18"/>
       <c r="O22" s="18"/>
@@ -2128,14 +2113,14 @@
       <c r="Z22" s="18"/>
     </row>
     <row r="23" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
+      <c r="A23" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="18"/>
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
@@ -2160,10 +2145,10 @@
       <c r="Z23" s="18"/>
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="26"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="30"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="28"/>
+      <c r="C24" s="28"/>
+      <c r="D24" s="28"/>
       <c r="E24" s="18"/>
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
@@ -2188,10 +2173,10 @@
       <c r="Z24" s="18"/>
     </row>
     <row r="25" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="26"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
+      <c r="A25" s="25"/>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
       <c r="E25" s="18"/>
       <c r="F25" s="18"/>
       <c r="G25" s="18"/>
@@ -2216,14 +2201,14 @@
       <c r="Z25" s="18"/>
     </row>
     <row r="26" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="A26" s="25" t="s">
+        <v>73</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
       <c r="E26" s="18"/>
       <c r="F26" s="18"/>
       <c r="G26" s="18"/>
@@ -2248,10 +2233,12 @@
       <c r="Z26" s="18"/>
     </row>
     <row r="27" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="26"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="30"/>
+      <c r="A27" s="25"/>
+      <c r="B27" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
       <c r="E27" s="18"/>
       <c r="F27" s="18"/>
       <c r="G27" s="18"/>
@@ -2276,10 +2263,10 @@
       <c r="Z27" s="18"/>
     </row>
     <row r="28" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="26"/>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="28"/>
+      <c r="C28" s="28"/>
+      <c r="D28" s="28"/>
       <c r="E28" s="18"/>
       <c r="F28" s="18"/>
       <c r="G28" s="18"/>
@@ -2304,14 +2291,14 @@
       <c r="Z28" s="18"/>
     </row>
     <row r="29" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="B29" s="31">
+      <c r="A29" s="25" t="s">
+        <v>74</v>
+      </c>
+      <c r="B29" s="29">
         <v>1</v>
       </c>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28"/>
       <c r="E29" s="18"/>
       <c r="F29" s="18"/>
       <c r="G29" s="18"/>
@@ -2336,16 +2323,16 @@
       <c r="Z29" s="18"/>
     </row>
     <row r="30" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="B30" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="33"/>
+      <c r="A30" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="B30" s="35" t="s">
+        <v>76</v>
+      </c>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="30"/>
+      <c r="F30" s="30"/>
       <c r="G30" s="18"/>
       <c r="H30" s="18"/>
       <c r="I30" s="18"/>
@@ -2368,16 +2355,16 @@
       <c r="Z30" s="18"/>
     </row>
     <row r="31" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="27"/>
-      <c r="D31" s="27"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="33"/>
+      <c r="A31" s="25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="30"/>
+      <c r="F31" s="30"/>
       <c r="G31" s="18"/>
       <c r="H31" s="18"/>
       <c r="I31" s="18"/>
@@ -2400,12 +2387,12 @@
       <c r="Z31" s="18"/>
     </row>
     <row r="32" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="34"/>
-      <c r="B32" s="35" t="s">
-        <v>83</v>
-      </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="34"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
       <c r="E32" s="18"/>
       <c r="F32" s="18"/>
       <c r="G32" s="18"/>
@@ -4306,7 +4293,7 @@
       <c r="Z99" s="18"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="A16:D16"/>
     <mergeCell ref="B19:D19"/>
@@ -4314,6 +4301,7 @@
     <mergeCell ref="B23:D23"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B27:D27"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B30" r:id="rId1" xr:uid="{F3C2EAD7-7A50-4580-BA7B-D7863331157E}"/>
@@ -4333,7 +4321,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H27" sqref="H27"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -5101,7 +5088,6 @@
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>